<commit_message>
Page Object Model Framework
</commit_message>
<xml_diff>
--- a/TestCase_Scenarios.xlsx
+++ b/TestCase_Scenarios.xlsx
@@ -9,13 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Home" sheetId="2" r:id="rId1"/>
-    <sheet name="Login" sheetId="3" r:id="rId2"/>
-    <sheet name="MyAccount" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Comman verification" sheetId="6" r:id="rId1"/>
+    <sheet name="Home" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="MyAccount" sheetId="1" r:id="rId4"/>
+    <sheet name="Products Details" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="8" r:id="rId6"/>
+    <sheet name="Order History" sheetId="4" r:id="rId7"/>
+    <sheet name="Address" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Check if Cart is empty after login.</t>
   </si>
@@ -35,9 +39,6 @@
     <t>Check Women, Dresses, Tshirt Header is displaying on each page.</t>
   </si>
   <si>
-    <t>Check Logo</t>
-  </si>
-  <si>
     <t>Search Sleevs &amp; Verify result.</t>
   </si>
   <si>
@@ -60,6 +61,63 @@
   </si>
   <si>
     <t>Verify all labels in MyAccount Section</t>
+  </si>
+  <si>
+    <t>Verify Address is same as entered.</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Can be done using JDBC connector of read from file</t>
+  </si>
+  <si>
+    <t>Verify user can update address</t>
+  </si>
+  <si>
+    <t>Verify user can delete address</t>
+  </si>
+  <si>
+    <t>Add a new address &amp; verify its displayed.</t>
+  </si>
+  <si>
+    <t>Go back to Account using "Back to your account"</t>
+  </si>
+  <si>
+    <t>Go back to Home page using "Home"</t>
+  </si>
+  <si>
+    <t>Verify Comman verification points</t>
+  </si>
+  <si>
+    <t>Verify Order History for user with no orders</t>
+  </si>
+  <si>
+    <t>Craete a order &amp; verify history.</t>
+  </si>
+  <si>
+    <t>Verifu Mouse hover on Women / Dresses / T-Shirts</t>
+  </si>
+  <si>
+    <t>verify Tooltip on mousehover</t>
+  </si>
+  <si>
+    <t>Verify price on mouse hover on a item</t>
+  </si>
+  <si>
+    <t>Add Item to Cart &amp; Verify count in Cart</t>
+  </si>
+  <si>
+    <t>MouseHover on cart &amp; verify item in cart</t>
+  </si>
+  <si>
+    <t>Verify total in cart after addign multiple items</t>
+  </si>
+  <si>
+    <t>Verify end to end order process while not logegd in</t>
+  </si>
+  <si>
+    <t>Verify end to end order process while not logegdin</t>
   </si>
 </sst>
 </file>
@@ -386,33 +444,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -425,25 +522,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -451,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -459,12 +556,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,23 +572,25 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>0</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,12 +600,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -515,16 +609,197 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test Case Scenarios for AUT.
</commit_message>
<xml_diff>
--- a/TestCase_Scenarios.xlsx
+++ b/TestCase_Scenarios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Comman verification" sheetId="6" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="Login" sheetId="3" r:id="rId3"/>
     <sheet name="MyAccount" sheetId="1" r:id="rId4"/>
     <sheet name="Products Details" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="8" r:id="rId6"/>
-    <sheet name="Order History" sheetId="4" r:id="rId7"/>
+    <sheet name="Order History" sheetId="4" r:id="rId6"/>
+    <sheet name="Shopping Cart" sheetId="9" r:id="rId7"/>
     <sheet name="Address" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
   <si>
     <t>Check if Cart is empty after login.</t>
   </si>
@@ -161,9 +161,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,130 +452,17 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="35.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -580,168 +472,38 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>9</v>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="60" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -759,43 +521,356 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="60" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="47" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="24.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Page Object Model Framework updated 12/16/2016
</commit_message>
<xml_diff>
--- a/TestCase_Scenarios.xlsx
+++ b/TestCase_Scenarios.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frameworks\Selenium_Training_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Comman verification" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Shopping Cart" sheetId="9" r:id="rId7"/>
     <sheet name="Address" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Check if Cart is empty after login.</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Verify Logo</t>
   </si>
   <si>
-    <t>Login Page verification</t>
-  </si>
-  <si>
     <t>Verify all labels in MyAccount Section</t>
   </si>
   <si>
@@ -118,6 +115,18 @@
   </si>
   <si>
     <t>Verify end to end order process while not logegdin</t>
+  </si>
+  <si>
+    <t>Verify Login page.</t>
+  </si>
+  <si>
+    <t>Verify use can crate an account.</t>
+  </si>
+  <si>
+    <t>Valid login scenario.</t>
+  </si>
+  <si>
+    <t>Invalid login scenarios.</t>
   </si>
 </sst>
 </file>
@@ -229,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,7 +273,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +471,7 @@
     <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -473,7 +482,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -493,10 +502,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,22 +526,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -542,21 +536,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -567,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -576,6 +570,29 @@
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -588,10 +605,10 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -610,14 +627,14 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,7 +649,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -643,13 +660,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G5"/>
+      <selection activeCell="C5" sqref="C5:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="47" style="2" bestFit="1" customWidth="1"/>
@@ -657,7 +674,7 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -668,47 +685,22 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -721,10 +713,10 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -743,22 +735,22 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -768,17 +760,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="24.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -794,7 +786,32 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -807,11 +824,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="32.140625" style="2" bestFit="1" customWidth="1"/>
@@ -819,7 +836,7 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -830,48 +847,48 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>